<commit_message>
fix column typo Marker_2 to marker_2 in biosample 3275
</commit_message>
<xml_diff>
--- a/bioSample/bioSample_3275.xlsx
+++ b/bioSample/bioSample_3275.xlsx
@@ -52,7 +52,7 @@
     <t xml:space="preserve">marker_1</t>
   </si>
   <si>
-    <t xml:space="preserve">Marker_2</t>
+    <t xml:space="preserve">marker_2</t>
   </si>
   <si>
     <t xml:space="preserve">08.09.18</t>
@@ -263,7 +263,7 @@
   <dimension ref="A1:K34"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J31" activeCellId="0" sqref="J31"/>
+      <selection pane="topLeft" activeCell="K1" activeCellId="0" sqref="K1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
corrected 37C.CO2 to DMEM.37C.C02
</commit_message>
<xml_diff>
--- a/bioSample/bioSample_3275.xlsx
+++ b/bioSample/bioSample_3275.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hollybrown/database_files/bioSample/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D2065D0-4155-E84C-BF5C-5D2465AD19B4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33F5A5B9-9CF6-B945-AF4C-2CD14FA0FA0F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="17700" yWindow="460" windowWidth="15900" windowHeight="18940" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="bioSample_3275" sheetId="1" r:id="rId1"/>
@@ -539,8 +539,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J49" sqref="J49"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I35" sqref="I35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -1634,6 +1634,9 @@
       <c r="H35">
         <v>90</v>
       </c>
+      <c r="I35">
+        <v>8</v>
+      </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A36" t="s">
@@ -1660,6 +1663,9 @@
       <c r="H36">
         <v>90</v>
       </c>
+      <c r="I36">
+        <v>7</v>
+      </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A37" t="s">
@@ -1685,6 +1691,9 @@
       </c>
       <c r="H37">
         <v>90</v>
+      </c>
+      <c r="I37">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated fastq files and related metadata
</commit_message>
<xml_diff>
--- a/bioSample/bioSample_3275.xlsx
+++ b/bioSample/bioSample_3275.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hollybrown/database_files/bioSample/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33F5A5B9-9CF6-B945-AF4C-2CD14FA0FA0F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DDFD295-B402-E246-AA8F-107A65C5A199}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17700" yWindow="460" windowWidth="15900" windowHeight="18940" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="bioSample_3275" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="62">
   <si>
     <t>harvestDate</t>
   </si>
@@ -75,9 +75,6 @@
     <t>CNAG_00000</t>
   </si>
   <si>
-    <t>37C.CO2</t>
-  </si>
-  <si>
     <t>10.15.18</t>
   </si>
   <si>
@@ -187,6 +184,33 @@
   </si>
   <si>
     <t>CNAG_00156</t>
+  </si>
+  <si>
+    <t>DMEM.37C.CO2</t>
+  </si>
+  <si>
+    <t>TDY2205</t>
+  </si>
+  <si>
+    <t>CNAG_06871</t>
+  </si>
+  <si>
+    <t>TDY1452</t>
+  </si>
+  <si>
+    <t>CNAG_02566</t>
+  </si>
+  <si>
+    <t>TDY1118</t>
+  </si>
+  <si>
+    <t>CNAG_05222</t>
+  </si>
+  <si>
+    <t>TDY1174</t>
+  </si>
+  <si>
+    <t>CNAG_00871</t>
   </si>
 </sst>
 </file>
@@ -537,10 +561,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K37"/>
+  <dimension ref="A1:K41"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I35" sqref="I35"/>
+      <selection sqref="A1:K1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -612,7 +636,7 @@
         <v>15</v>
       </c>
       <c r="G2" t="s">
-        <v>16</v>
+        <v>53</v>
       </c>
       <c r="H2">
         <v>90</v>
@@ -623,7 +647,7 @@
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B3" t="s">
         <v>12</v>
@@ -641,7 +665,7 @@
         <v>15</v>
       </c>
       <c r="G3" t="s">
-        <v>16</v>
+        <v>53</v>
       </c>
       <c r="H3">
         <v>90</v>
@@ -652,7 +676,7 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B4" t="s">
         <v>12</v>
@@ -670,7 +694,7 @@
         <v>15</v>
       </c>
       <c r="G4" t="s">
-        <v>16</v>
+        <v>53</v>
       </c>
       <c r="H4">
         <v>90</v>
@@ -681,7 +705,7 @@
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B5" t="s">
         <v>12</v>
@@ -693,13 +717,13 @@
         <v>13</v>
       </c>
       <c r="E5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F5" t="s">
         <v>19</v>
       </c>
-      <c r="F5" t="s">
-        <v>20</v>
-      </c>
       <c r="G5" t="s">
-        <v>16</v>
+        <v>53</v>
       </c>
       <c r="H5">
         <v>90</v>
@@ -710,7 +734,7 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B6" t="s">
         <v>12</v>
@@ -722,13 +746,13 @@
         <v>13</v>
       </c>
       <c r="E6" t="s">
+        <v>18</v>
+      </c>
+      <c r="F6" t="s">
         <v>19</v>
       </c>
-      <c r="F6" t="s">
-        <v>20</v>
-      </c>
       <c r="G6" t="s">
-        <v>16</v>
+        <v>53</v>
       </c>
       <c r="H6">
         <v>90</v>
@@ -739,7 +763,7 @@
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B7" t="s">
         <v>12</v>
@@ -751,13 +775,13 @@
         <v>13</v>
       </c>
       <c r="E7" t="s">
+        <v>20</v>
+      </c>
+      <c r="F7" t="s">
         <v>21</v>
       </c>
-      <c r="F7" t="s">
-        <v>22</v>
-      </c>
       <c r="G7" t="s">
-        <v>16</v>
+        <v>53</v>
       </c>
       <c r="H7">
         <v>90</v>
@@ -768,7 +792,7 @@
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B8" t="s">
         <v>12</v>
@@ -780,13 +804,13 @@
         <v>13</v>
       </c>
       <c r="E8" t="s">
+        <v>22</v>
+      </c>
+      <c r="F8" t="s">
         <v>23</v>
       </c>
-      <c r="F8" t="s">
-        <v>24</v>
-      </c>
       <c r="G8" t="s">
-        <v>16</v>
+        <v>53</v>
       </c>
       <c r="H8">
         <v>90</v>
@@ -795,12 +819,12 @@
         <v>4</v>
       </c>
       <c r="J8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B9" t="s">
         <v>12</v>
@@ -812,13 +836,13 @@
         <v>13</v>
       </c>
       <c r="E9" t="s">
+        <v>22</v>
+      </c>
+      <c r="F9" t="s">
         <v>23</v>
       </c>
-      <c r="F9" t="s">
-        <v>24</v>
-      </c>
       <c r="G9" t="s">
-        <v>16</v>
+        <v>53</v>
       </c>
       <c r="H9">
         <v>90</v>
@@ -827,7 +851,7 @@
         <v>5</v>
       </c>
       <c r="J9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.15">
@@ -844,13 +868,13 @@
         <v>13</v>
       </c>
       <c r="E10" t="s">
+        <v>26</v>
+      </c>
+      <c r="F10" t="s">
         <v>27</v>
       </c>
-      <c r="F10" t="s">
-        <v>28</v>
-      </c>
       <c r="G10" t="s">
-        <v>16</v>
+        <v>53</v>
       </c>
       <c r="H10">
         <v>90</v>
@@ -861,7 +885,7 @@
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A11" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B11" t="s">
         <v>12</v>
@@ -873,13 +897,13 @@
         <v>13</v>
       </c>
       <c r="E11" t="s">
+        <v>26</v>
+      </c>
+      <c r="F11" t="s">
         <v>27</v>
       </c>
-      <c r="F11" t="s">
-        <v>28</v>
-      </c>
       <c r="G11" t="s">
-        <v>16</v>
+        <v>53</v>
       </c>
       <c r="H11">
         <v>90</v>
@@ -890,25 +914,25 @@
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A12" t="s">
+        <v>25</v>
+      </c>
+      <c r="B12" t="s">
+        <v>12</v>
+      </c>
+      <c r="C12">
+        <v>12</v>
+      </c>
+      <c r="D12" t="s">
+        <v>13</v>
+      </c>
+      <c r="E12" t="s">
         <v>26</v>
       </c>
-      <c r="B12" t="s">
-        <v>12</v>
-      </c>
-      <c r="C12">
-        <v>12</v>
-      </c>
-      <c r="D12" t="s">
-        <v>13</v>
-      </c>
-      <c r="E12" t="s">
+      <c r="F12" t="s">
         <v>27</v>
       </c>
-      <c r="F12" t="s">
-        <v>28</v>
-      </c>
       <c r="G12" t="s">
-        <v>16</v>
+        <v>53</v>
       </c>
       <c r="H12">
         <v>90</v>
@@ -931,13 +955,13 @@
         <v>13</v>
       </c>
       <c r="E13" t="s">
+        <v>28</v>
+      </c>
+      <c r="F13" t="s">
         <v>29</v>
       </c>
-      <c r="F13" t="s">
-        <v>30</v>
-      </c>
       <c r="G13" t="s">
-        <v>16</v>
+        <v>53</v>
       </c>
       <c r="H13">
         <v>90</v>
@@ -946,15 +970,15 @@
         <v>5</v>
       </c>
       <c r="J13" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="K13" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A14" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B14" t="s">
         <v>12</v>
@@ -966,13 +990,13 @@
         <v>13</v>
       </c>
       <c r="E14" t="s">
+        <v>28</v>
+      </c>
+      <c r="F14" t="s">
         <v>29</v>
       </c>
-      <c r="F14" t="s">
-        <v>30</v>
-      </c>
       <c r="G14" t="s">
-        <v>16</v>
+        <v>53</v>
       </c>
       <c r="H14">
         <v>90</v>
@@ -981,15 +1005,15 @@
         <v>6</v>
       </c>
       <c r="J14" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="K14" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A15" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B15" t="s">
         <v>12</v>
@@ -1001,13 +1025,13 @@
         <v>13</v>
       </c>
       <c r="E15" t="s">
+        <v>28</v>
+      </c>
+      <c r="F15" t="s">
         <v>29</v>
       </c>
-      <c r="F15" t="s">
-        <v>30</v>
-      </c>
       <c r="G15" t="s">
-        <v>16</v>
+        <v>53</v>
       </c>
       <c r="H15">
         <v>90</v>
@@ -1016,15 +1040,15 @@
         <v>7</v>
       </c>
       <c r="J15" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="K15" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A16" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B16" t="s">
         <v>12</v>
@@ -1036,13 +1060,13 @@
         <v>13</v>
       </c>
       <c r="E16" t="s">
+        <v>28</v>
+      </c>
+      <c r="F16" t="s">
         <v>29</v>
       </c>
-      <c r="F16" t="s">
-        <v>30</v>
-      </c>
       <c r="G16" t="s">
-        <v>16</v>
+        <v>53</v>
       </c>
       <c r="H16">
         <v>90</v>
@@ -1051,10 +1075,10 @@
         <v>8</v>
       </c>
       <c r="J16" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="K16" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.15">
@@ -1071,13 +1095,13 @@
         <v>13</v>
       </c>
       <c r="E17" t="s">
+        <v>31</v>
+      </c>
+      <c r="F17" t="s">
         <v>32</v>
       </c>
-      <c r="F17" t="s">
-        <v>33</v>
-      </c>
       <c r="G17" t="s">
-        <v>16</v>
+        <v>53</v>
       </c>
       <c r="H17">
         <v>90</v>
@@ -1086,12 +1110,12 @@
         <v>4</v>
       </c>
       <c r="J17" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A18" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B18" t="s">
         <v>12</v>
@@ -1103,13 +1127,13 @@
         <v>13</v>
       </c>
       <c r="E18" t="s">
+        <v>31</v>
+      </c>
+      <c r="F18" t="s">
         <v>32</v>
       </c>
-      <c r="F18" t="s">
-        <v>33</v>
-      </c>
       <c r="G18" t="s">
-        <v>16</v>
+        <v>53</v>
       </c>
       <c r="H18">
         <v>90</v>
@@ -1118,12 +1142,12 @@
         <v>5</v>
       </c>
       <c r="J18" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A19" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B19" t="s">
         <v>12</v>
@@ -1135,13 +1159,13 @@
         <v>13</v>
       </c>
       <c r="E19" t="s">
+        <v>31</v>
+      </c>
+      <c r="F19" t="s">
         <v>32</v>
       </c>
-      <c r="F19" t="s">
-        <v>33</v>
-      </c>
       <c r="G19" t="s">
-        <v>16</v>
+        <v>53</v>
       </c>
       <c r="H19">
         <v>90</v>
@@ -1150,7 +1174,7 @@
         <v>6</v>
       </c>
       <c r="J19" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.15">
@@ -1167,13 +1191,13 @@
         <v>13</v>
       </c>
       <c r="E20" t="s">
+        <v>33</v>
+      </c>
+      <c r="F20" t="s">
         <v>34</v>
       </c>
-      <c r="F20" t="s">
-        <v>35</v>
-      </c>
       <c r="G20" t="s">
-        <v>16</v>
+        <v>53</v>
       </c>
       <c r="H20">
         <v>90</v>
@@ -1184,7 +1208,7 @@
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A21" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B21" t="s">
         <v>12</v>
@@ -1196,13 +1220,13 @@
         <v>13</v>
       </c>
       <c r="E21" t="s">
+        <v>33</v>
+      </c>
+      <c r="F21" t="s">
         <v>34</v>
       </c>
-      <c r="F21" t="s">
-        <v>35</v>
-      </c>
       <c r="G21" t="s">
-        <v>16</v>
+        <v>53</v>
       </c>
       <c r="H21">
         <v>90</v>
@@ -1213,7 +1237,7 @@
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A22" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B22" t="s">
         <v>12</v>
@@ -1225,13 +1249,13 @@
         <v>13</v>
       </c>
       <c r="E22" t="s">
+        <v>35</v>
+      </c>
+      <c r="F22" t="s">
         <v>36</v>
       </c>
-      <c r="F22" t="s">
-        <v>37</v>
-      </c>
       <c r="G22" t="s">
-        <v>16</v>
+        <v>53</v>
       </c>
       <c r="H22">
         <v>90</v>
@@ -1240,12 +1264,12 @@
         <v>7</v>
       </c>
       <c r="J22" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A23" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B23" t="s">
         <v>12</v>
@@ -1257,13 +1281,13 @@
         <v>13</v>
       </c>
       <c r="E23" t="s">
+        <v>35</v>
+      </c>
+      <c r="F23" t="s">
         <v>36</v>
       </c>
-      <c r="F23" t="s">
-        <v>37</v>
-      </c>
       <c r="G23" t="s">
-        <v>16</v>
+        <v>53</v>
       </c>
       <c r="H23">
         <v>90</v>
@@ -1272,12 +1296,12 @@
         <v>8</v>
       </c>
       <c r="J23" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A24" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B24" t="s">
         <v>12</v>
@@ -1289,13 +1313,13 @@
         <v>13</v>
       </c>
       <c r="E24" t="s">
+        <v>37</v>
+      </c>
+      <c r="F24" t="s">
         <v>38</v>
       </c>
-      <c r="F24" t="s">
-        <v>39</v>
-      </c>
       <c r="G24" t="s">
-        <v>16</v>
+        <v>53</v>
       </c>
       <c r="H24">
         <v>90</v>
@@ -1304,7 +1328,7 @@
         <v>1</v>
       </c>
       <c r="J24" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.15">
@@ -1321,13 +1345,13 @@
         <v>13</v>
       </c>
       <c r="E25" t="s">
+        <v>39</v>
+      </c>
+      <c r="F25" t="s">
         <v>40</v>
       </c>
-      <c r="F25" t="s">
-        <v>41</v>
-      </c>
       <c r="G25" t="s">
-        <v>16</v>
+        <v>53</v>
       </c>
       <c r="H25">
         <v>90</v>
@@ -1338,7 +1362,7 @@
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A26" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B26" t="s">
         <v>12</v>
@@ -1350,13 +1374,13 @@
         <v>13</v>
       </c>
       <c r="E26" t="s">
+        <v>39</v>
+      </c>
+      <c r="F26" t="s">
         <v>40</v>
       </c>
-      <c r="F26" t="s">
-        <v>41</v>
-      </c>
       <c r="G26" t="s">
-        <v>16</v>
+        <v>53</v>
       </c>
       <c r="H26">
         <v>90</v>
@@ -1367,7 +1391,7 @@
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A27" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B27" t="s">
         <v>12</v>
@@ -1379,13 +1403,13 @@
         <v>13</v>
       </c>
       <c r="E27" t="s">
+        <v>39</v>
+      </c>
+      <c r="F27" t="s">
         <v>40</v>
       </c>
-      <c r="F27" t="s">
-        <v>41</v>
-      </c>
       <c r="G27" t="s">
-        <v>16</v>
+        <v>53</v>
       </c>
       <c r="H27">
         <v>90</v>
@@ -1408,13 +1432,13 @@
         <v>13</v>
       </c>
       <c r="E28" t="s">
+        <v>41</v>
+      </c>
+      <c r="F28" t="s">
         <v>42</v>
       </c>
-      <c r="F28" t="s">
-        <v>43</v>
-      </c>
       <c r="G28" t="s">
-        <v>16</v>
+        <v>53</v>
       </c>
       <c r="H28">
         <v>90</v>
@@ -1423,12 +1447,12 @@
         <v>4</v>
       </c>
       <c r="J28" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A29" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B29" t="s">
         <v>12</v>
@@ -1440,13 +1464,13 @@
         <v>13</v>
       </c>
       <c r="E29" t="s">
+        <v>41</v>
+      </c>
+      <c r="F29" t="s">
         <v>42</v>
       </c>
-      <c r="F29" t="s">
-        <v>43</v>
-      </c>
       <c r="G29" t="s">
-        <v>16</v>
+        <v>53</v>
       </c>
       <c r="H29">
         <v>90</v>
@@ -1455,12 +1479,12 @@
         <v>5</v>
       </c>
       <c r="J29" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A30" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B30" t="s">
         <v>12</v>
@@ -1472,13 +1496,13 @@
         <v>13</v>
       </c>
       <c r="E30" t="s">
+        <v>41</v>
+      </c>
+      <c r="F30" t="s">
         <v>42</v>
       </c>
-      <c r="F30" t="s">
-        <v>43</v>
-      </c>
       <c r="G30" t="s">
-        <v>16</v>
+        <v>53</v>
       </c>
       <c r="H30">
         <v>90</v>
@@ -1487,12 +1511,12 @@
         <v>6</v>
       </c>
       <c r="J30" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A31" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B31" t="s">
         <v>12</v>
@@ -1504,13 +1528,13 @@
         <v>13</v>
       </c>
       <c r="E31" t="s">
+        <v>43</v>
+      </c>
+      <c r="F31" t="s">
         <v>44</v>
       </c>
-      <c r="F31" t="s">
-        <v>45</v>
-      </c>
       <c r="G31" t="s">
-        <v>16</v>
+        <v>53</v>
       </c>
       <c r="H31">
         <v>90</v>
@@ -1519,12 +1543,12 @@
         <v>6</v>
       </c>
       <c r="J31" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A32" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B32" t="s">
         <v>12</v>
@@ -1542,7 +1566,7 @@
         <v>15</v>
       </c>
       <c r="G32" t="s">
-        <v>16</v>
+        <v>53</v>
       </c>
       <c r="H32">
         <v>90</v>
@@ -1553,7 +1577,7 @@
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A33" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B33" t="s">
         <v>12</v>
@@ -1565,13 +1589,13 @@
         <v>13</v>
       </c>
       <c r="E33" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F33" t="s">
         <v>15</v>
       </c>
       <c r="G33" t="s">
-        <v>16</v>
+        <v>53</v>
       </c>
       <c r="H33">
         <v>90</v>
@@ -1582,7 +1606,7 @@
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A34" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B34" t="s">
         <v>12</v>
@@ -1594,13 +1618,13 @@
         <v>13</v>
       </c>
       <c r="E34" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F34" t="s">
         <v>15</v>
       </c>
       <c r="G34" t="s">
-        <v>16</v>
+        <v>53</v>
       </c>
       <c r="H34">
         <v>90</v>
@@ -1623,13 +1647,13 @@
         <v>13</v>
       </c>
       <c r="E35" t="s">
+        <v>47</v>
+      </c>
+      <c r="F35" t="s">
         <v>48</v>
       </c>
-      <c r="F35" t="s">
-        <v>49</v>
-      </c>
       <c r="G35" t="s">
-        <v>16</v>
+        <v>53</v>
       </c>
       <c r="H35">
         <v>90</v>
@@ -1640,7 +1664,7 @@
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A36" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B36" t="s">
         <v>12</v>
@@ -1652,13 +1676,13 @@
         <v>13</v>
       </c>
       <c r="E36" t="s">
+        <v>49</v>
+      </c>
+      <c r="F36" t="s">
         <v>50</v>
       </c>
-      <c r="F36" t="s">
-        <v>51</v>
-      </c>
       <c r="G36" t="s">
-        <v>16</v>
+        <v>53</v>
       </c>
       <c r="H36">
         <v>90</v>
@@ -1669,7 +1693,7 @@
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A37" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B37" t="s">
         <v>12</v>
@@ -1681,19 +1705,135 @@
         <v>13</v>
       </c>
       <c r="E37" t="s">
+        <v>51</v>
+      </c>
+      <c r="F37" t="s">
         <v>52</v>
       </c>
-      <c r="F37" t="s">
-        <v>53</v>
-      </c>
       <c r="G37" t="s">
-        <v>16</v>
+        <v>53</v>
       </c>
       <c r="H37">
         <v>90</v>
       </c>
       <c r="I37">
         <v>7</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A38" t="s">
+        <v>11</v>
+      </c>
+      <c r="B38" t="s">
+        <v>12</v>
+      </c>
+      <c r="C38">
+        <v>38</v>
+      </c>
+      <c r="D38" t="s">
+        <v>13</v>
+      </c>
+      <c r="E38" t="s">
+        <v>54</v>
+      </c>
+      <c r="F38" t="s">
+        <v>55</v>
+      </c>
+      <c r="G38" t="s">
+        <v>53</v>
+      </c>
+      <c r="H38">
+        <v>90</v>
+      </c>
+      <c r="I38">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A39" t="s">
+        <v>16</v>
+      </c>
+      <c r="B39" t="s">
+        <v>12</v>
+      </c>
+      <c r="C39">
+        <v>39</v>
+      </c>
+      <c r="D39" t="s">
+        <v>13</v>
+      </c>
+      <c r="E39" t="s">
+        <v>56</v>
+      </c>
+      <c r="F39" t="s">
+        <v>57</v>
+      </c>
+      <c r="G39" t="s">
+        <v>53</v>
+      </c>
+      <c r="H39">
+        <v>90</v>
+      </c>
+      <c r="I39">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A40" t="s">
+        <v>25</v>
+      </c>
+      <c r="B40" t="s">
+        <v>12</v>
+      </c>
+      <c r="C40">
+        <v>40</v>
+      </c>
+      <c r="D40" t="s">
+        <v>13</v>
+      </c>
+      <c r="E40" t="s">
+        <v>58</v>
+      </c>
+      <c r="F40" t="s">
+        <v>59</v>
+      </c>
+      <c r="G40" t="s">
+        <v>53</v>
+      </c>
+      <c r="H40">
+        <v>90</v>
+      </c>
+      <c r="I40">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A41" t="s">
+        <v>16</v>
+      </c>
+      <c r="B41" t="s">
+        <v>12</v>
+      </c>
+      <c r="C41">
+        <v>41</v>
+      </c>
+      <c r="D41" t="s">
+        <v>13</v>
+      </c>
+      <c r="E41" t="s">
+        <v>60</v>
+      </c>
+      <c r="F41" t="s">
+        <v>61</v>
+      </c>
+      <c r="G41" t="s">
+        <v>53</v>
+      </c>
+      <c r="H41">
+        <v>90</v>
+      </c>
+      <c r="I41">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>